<commit_message>
Changes to account lookup test data
</commit_message>
<xml_diff>
--- a/Test_Data/Account Lookup.xlsx
+++ b/Test_Data/Account Lookup.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/55cd0139eebd0c53/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/55cd0139eebd0c53/Desktop/Finance Automations/Finance-Automation/Test_Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="30" documentId="8_{CB1126F0-84BB-4F77-9345-DCA14FCEAEFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AE9210A1-8194-4CDE-B862-8F59ABF8E3FC}"/>
+  <xr:revisionPtr revIDLastSave="32" documentId="8_{CB1126F0-84BB-4F77-9345-DCA14FCEAEFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D685264F-050F-4C63-BD55-3E34178B129C}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-5010" windowWidth="29040" windowHeight="15720" xr2:uid="{EF4987E2-0364-45BC-8B6A-A4DF90DF85D0}"/>
+    <workbookView xWindow="57480" yWindow="-5010" windowWidth="29040" windowHeight="15720" xr2:uid="{EF4987E2-0364-45BC-8B6A-A4DF90DF85D0}"/>
   </bookViews>
   <sheets>
     <sheet name="Account Lookup" sheetId="1" r:id="rId1"/>
@@ -915,13 +915,12 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="19.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">

</xml_diff>